<commit_message>
version 0.0.1 - Jun 2020
</commit_message>
<xml_diff>
--- a/StructureDefinition-hla-allele.xlsx
+++ b/StructureDefinition-hla-allele.xlsx
@@ -1643,48 +1643,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="45.3515625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="23.79296875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="40.90625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.07421875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="43.60546875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="21.7421875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="255.0" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="65.8984375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="66.86328125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="22.18359375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="41.59375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="60.51953125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="61.7109375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="21.72265625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.81640625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.21484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="24.81640625" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="26.57421875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="23.20703125" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="26.71484375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="239.703125" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="109.91015625" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="33.046875" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="38.60546875" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="103.87890625" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="32.84375" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="37.70703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>